<commit_message>
atualização feita pelo Thiago
</commit_message>
<xml_diff>
--- a/docs/sprint_backlog_2.xlsx
+++ b/docs/sprint_backlog_2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="850" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="850" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="01 - Product Backlog" sheetId="1" r:id="rId1"/>
@@ -15,6 +15,15 @@
     <sheet name="Tarefas Sprint 2" sheetId="6" r:id="rId6"/>
     <sheet name="User Stories" sheetId="7" r:id="rId7"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'01 - Product Backlog'!$A$1:$E$28</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'02 - Planejamento Sprint 1'!$A$1:$E$28</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'02 - Tarefas de gerenciamento'!$A$1:$D$11</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">'03 - Tarefas Sprint 1'!$A$1:$E$43</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">'Planejamento Sprint 2'!$A$1:$E$31</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="5">'Tarefas Sprint 2'!$A$1:$E$26</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="6">'User Stories'!$A$1:$C$26</definedName>
+  </definedNames>
   <calcPr calcId="145621" iterateDelta="1E-4"/>
 </workbook>
 </file>
@@ -374,35 +383,35 @@
     <t>Total de horas alocadas</t>
   </si>
   <si>
-    <t>** Como não há base histórica para a capacidade da equipe em relação ao tamanho das funcionalidades, estipulou-se três horas por ponto. 
+    <t>Percentual de alocação da equipe</t>
+  </si>
+  <si>
+    <t>Lições aprendidas</t>
+  </si>
+  <si>
+    <t>Reunião de lições aprendidas</t>
+  </si>
+  <si>
+    <t>TT - Deve-se implementar uma nova tela que permita informar o ano e os feriados do ano. Estes feriados devem ser abonados de todos os funcionários</t>
+  </si>
+  <si>
+    <t>Atividades de gerenciamento do projeto</t>
+  </si>
+  <si>
+    <t>Coeficiente para resposta a riscos (10%)</t>
+  </si>
+  <si>
+    <t>Gerenciamento do projeto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reuniões </t>
+  </si>
+  <si>
+    <t>~94%</t>
+  </si>
+  <si>
+    <t>** Como não há base histórica para a capacidade da equipe em relação ao tamanho das funcionalidades, estipulou-se duas horas por ponto. 
 Os testes considera-se 1/3 do tempo de desenvolvimento</t>
-  </si>
-  <si>
-    <t>Percentual de alocação da equipe</t>
-  </si>
-  <si>
-    <t>Lições aprendidas</t>
-  </si>
-  <si>
-    <t>Reunião de lições aprendidas</t>
-  </si>
-  <si>
-    <t>TT - Deve-se implementar uma nova tela que permita informar o ano e os feriados do ano. Estes feriados devem ser abonados de todos os funcionários</t>
-  </si>
-  <si>
-    <t>Atividades de gerenciamento do projeto</t>
-  </si>
-  <si>
-    <t>Coeficiente para resposta a riscos (10%)</t>
-  </si>
-  <si>
-    <t>~97%</t>
-  </si>
-  <si>
-    <t>Gerenciamento do projeto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reuniões </t>
   </si>
 </sst>
 </file>
@@ -577,12 +586,6 @@
   </cellStyleXfs>
   <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -622,18 +625,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -677,6 +668,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -754,6 +763,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1048,222 +1060,222 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D25"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="8.7109375"/>
     <col min="3" max="3" width="74"/>
-    <col min="4" max="4" width="17" style="3"/>
+    <col min="4" max="4" width="17" style="1"/>
     <col min="5" max="257" width="8.7109375"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="5" t="s">
+      <c r="C4" s="40"/>
+      <c r="D4" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="6">
+      <c r="B5" s="4">
         <v>1</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="6">
+      <c r="B6" s="4">
         <v>2</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="6">
+      <c r="B7" s="4">
         <v>3</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="6">
+      <c r="B8" s="4">
         <v>4</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="6">
+      <c r="B9" s="4">
         <v>5</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="4">
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="6">
+      <c r="B10" s="4">
         <v>6</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="4">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="6">
+      <c r="B11" s="4">
         <v>7</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="4">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B12" s="6">
+      <c r="B12" s="4">
         <v>8</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B13" s="6">
+      <c r="B13" s="4">
         <v>9</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="4">
         <v>6</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="6">
+      <c r="B14" s="4">
         <v>10</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="4">
         <v>6</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="6">
+      <c r="B15" s="4">
         <v>11</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="4">
         <v>6</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B16" s="6">
+      <c r="B16" s="4">
         <v>12</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="6">
+      <c r="B17" s="4">
         <v>13</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="4">
         <v>7</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B18" s="6">
+      <c r="B18" s="4">
         <v>14</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="4">
         <v>8</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="6"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="6"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="4"/>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="6"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="6"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="4"/>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="6"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="6"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="4"/>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="6"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="6"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="4"/>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="6"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="6"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="4"/>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="6"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="6"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="4"/>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="6"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="6"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1271,7 +1283,7 @@
     <mergeCell ref="B4:C4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1280,7 +1292,7 @@
   <dimension ref="B2:C10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1292,67 +1304,67 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="C2" s="39"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C3" s="3"/>
+      <c r="C3" s="1"/>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="4">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="9">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="9">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="9">
         <v>6</v>
       </c>
     </row>
@@ -1361,7 +1373,7 @@
     <mergeCell ref="B2:C2"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1370,178 +1382,178 @@
   <dimension ref="A2:D27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.7109375"/>
     <col min="2" max="2" width="50.42578125"/>
-    <col min="3" max="3" width="10.42578125" style="3"/>
-    <col min="4" max="4" width="12" style="3"/>
+    <col min="3" max="3" width="10.42578125" style="1"/>
+    <col min="4" max="4" width="12" style="1"/>
     <col min="5" max="257" width="8.7109375"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
+      <c r="A3" s="10"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="12" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="4">
         <v>1</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="4">
         <v>2</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="4">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="4">
         <v>3</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="4">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="7"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="7"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="7"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="7"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="7"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="7"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="7"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="7"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="7"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="7"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="7"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="7"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="7"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="7"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="7"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="7"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="7"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="7"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="7"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="7"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:D2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1549,8 +1561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D42"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1563,297 +1575,297 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="12" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="2">
         <v>1</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="14" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="14" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="14" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="14" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="2">
         <v>2</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="2">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="16">
+      <c r="D12" s="14">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="16">
+      <c r="D13" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="16">
+      <c r="D14" s="14">
         <v>3</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="16">
+      <c r="D15" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="7"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="2">
         <v>3</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="D18" s="16">
+      <c r="D18" s="14">
         <v>3</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="D19" s="16">
+      <c r="D19" s="14">
         <v>2</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="7"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="15"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="7"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="7"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="15"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="7"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="7"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="7"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="7"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="7"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="7"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="7"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="7"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="7"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="7"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="7"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B36" s="7"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B37" s="7"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B38" s="7"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B39" s="7"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B40" s="7"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B41" s="7"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B42" s="7"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:D2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1861,8 +1873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1875,204 +1887,204 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="A3" s="10"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="12" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="2">
         <v>1</v>
       </c>
-      <c r="D5" s="6">
-        <v>102</v>
-      </c>
-      <c r="F5" s="17"/>
+      <c r="D5" s="4">
+        <v>68</v>
+      </c>
+      <c r="F5" s="15"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="2">
         <v>1</v>
       </c>
-      <c r="D6" s="6">
-        <v>34</v>
+      <c r="D6" s="4">
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1</v>
+      </c>
+      <c r="D7" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="C8" s="19">
+        <v>2</v>
+      </c>
+      <c r="D8" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="C7" s="4">
-        <v>1</v>
-      </c>
-      <c r="D7" s="11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="27" t="s">
-        <v>116</v>
-      </c>
-      <c r="C8" s="21">
-        <v>2</v>
-      </c>
-      <c r="D8" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="27" t="s">
-        <v>120</v>
-      </c>
-      <c r="C9" s="21">
+      <c r="C9" s="19">
         <v>3</v>
       </c>
-      <c r="D9" s="11">
-        <v>17</v>
+      <c r="D9" s="9">
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="27"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="11"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="9"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="7"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="C12" s="22">
-        <v>169</v>
-      </c>
-      <c r="D12" s="23"/>
+      <c r="C12" s="41">
+        <v>126</v>
+      </c>
+      <c r="D12" s="42"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="C13" s="24">
-        <v>165</v>
-      </c>
-      <c r="D13" s="25"/>
+      <c r="C13" s="43">
+        <v>115</v>
+      </c>
+      <c r="D13" s="44"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="C14" s="22" t="s">
-        <v>121</v>
-      </c>
-      <c r="D14" s="23"/>
+      <c r="B14" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="C14" s="41" t="s">
+        <v>122</v>
+      </c>
+      <c r="D14" s="42"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="7"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="7"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="7"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="7"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="7"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="7"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="7"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="7"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="7"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="7"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="7"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="7"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="7"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="7"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="7"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="7"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2082,7 +2094,7 @@
     <mergeCell ref="C14:D14"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2090,8 +2102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2104,253 +2116,253 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="12" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="2">
         <v>1</v>
       </c>
-      <c r="D5" s="4">
-        <v>102</v>
+      <c r="D5" s="2">
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="16">
+      <c r="D6" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="14">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="16">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="14">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="16">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="D9" s="16">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="D10" s="6">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="D11" s="16">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="14">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="D12" s="16">
-        <v>9</v>
-      </c>
-    </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="16">
+      <c r="D13" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" s="14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" s="14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" s="14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="2">
+        <v>2</v>
+      </c>
+      <c r="D19" s="2">
+        <v>23</v>
+      </c>
+      <c r="F19" s="15"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="14">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="C21" s="19">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="D14" s="16">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="D15" s="16">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="D16" s="16">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="D17" s="16">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="D18" s="16">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="4">
+      <c r="D21" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="38" t="s">
+        <v>121</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="9">
+        <v>3</v>
+      </c>
+      <c r="G23" s="15"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="C24" s="2">
+        <v>4</v>
+      </c>
+      <c r="D24" s="2">
         <v>2</v>
       </c>
-      <c r="D19" s="4">
-        <v>34</v>
-      </c>
-      <c r="F19" s="17"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D20" s="16">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="27" t="s">
-        <v>119</v>
-      </c>
-      <c r="C21" s="21">
-        <v>3</v>
-      </c>
-      <c r="D21" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="26" t="s">
-        <v>122</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="D22" s="11">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="44" t="s">
-        <v>123</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="D23" s="11">
-        <v>3</v>
-      </c>
-      <c r="G23" s="17"/>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="15" t="s">
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="C24" s="4">
-        <v>4</v>
-      </c>
-      <c r="D24" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="26" t="s">
-        <v>117</v>
-      </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D25" s="11">
+      <c r="D25" s="9">
         <v>2</v>
       </c>
     </row>
@@ -2359,7 +2371,7 @@
     <mergeCell ref="B2:D2"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2367,8 +2379,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2380,240 +2392,240 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="B2" s="11">
+      <c r="B2" s="9">
         <v>4</v>
       </c>
-      <c r="C2" s="11">
+      <c r="C2" s="9">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="C3" s="11"/>
+      <c r="C3" s="9"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="C4" s="11"/>
+      <c r="C4" s="9"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="C5" s="11"/>
+      <c r="C5" s="9"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="B6" s="31">
+      <c r="B6" s="25">
         <v>5</v>
       </c>
-      <c r="C6" s="31">
+      <c r="C6" s="25">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="C7" s="31"/>
+      <c r="C7" s="25"/>
     </row>
     <row r="8" spans="1:3" ht="39" x14ac:dyDescent="0.25">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="C8" s="31"/>
+      <c r="C8" s="25"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B9" s="9">
         <v>7</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="9">
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="33" t="s">
+      <c r="A10" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="C10" s="11"/>
+      <c r="C10" s="9"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="B11" s="31">
+      <c r="B11" s="25">
         <v>8</v>
       </c>
-      <c r="C11" s="31">
+      <c r="C11" s="25">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="29" t="s">
         <v>91</v>
       </c>
-      <c r="B12" s="31" t="s">
+      <c r="B12" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="C12" s="31"/>
+      <c r="C12" s="25"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="B13" s="11">
+      <c r="B13" s="9">
         <v>9</v>
       </c>
-      <c r="C13" s="11">
+      <c r="C13" s="9">
         <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="36" t="s">
+      <c r="A14" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="C14" s="11"/>
+      <c r="C14" s="9"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="37" t="s">
+      <c r="A15" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="B15" s="31">
+      <c r="B15" s="25">
         <v>10</v>
       </c>
-      <c r="C15" s="31">
+      <c r="C15" s="25">
         <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="B16" s="31" t="s">
+      <c r="B16" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="C16" s="31"/>
+      <c r="C16" s="25"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="B17" s="11">
+      <c r="B17" s="9">
         <v>11</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C17" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="36" t="s">
+      <c r="A18" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="C18" s="11"/>
+      <c r="C18" s="9"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="B19" s="31">
+      <c r="B19" s="25">
         <v>12</v>
       </c>
-      <c r="C19" s="31">
+      <c r="C19" s="25">
         <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="35" t="s">
+      <c r="A20" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="B20" s="31" t="s">
+      <c r="B20" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="C20" s="31"/>
+      <c r="C20" s="25"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="B21" s="11">
+      <c r="B21" s="9">
         <v>6</v>
       </c>
-      <c r="C21" s="11">
+      <c r="C21" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="38" t="s">
+      <c r="A22" s="32" t="s">
         <v>106</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="C22" s="11"/>
+      <c r="C22" s="9"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="39" t="s">
+      <c r="A23" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="B23" s="40">
+      <c r="B23" s="34">
         <v>13</v>
       </c>
-      <c r="C23" s="41"/>
+      <c r="C23" s="35"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="42" t="s">
-        <v>118</v>
-      </c>
-      <c r="B24" s="43" t="s">
+      <c r="A24" s="36" t="s">
+        <v>117</v>
+      </c>
+      <c r="B24" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="C24" s="40">
+      <c r="C24" s="34">
         <v>3</v>
       </c>
     </row>
@@ -2623,15 +2635,15 @@
       </c>
     </row>
     <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="19" t="s">
-        <v>114</v>
+      <c r="A26" s="17" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="20"/>
+      <c r="A27" s="18"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="17"/>
+      <c r="A30" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>